<commit_message>
[Refator] MVP 패턴 적용
</commit_message>
<xml_diff>
--- a/Assets/Data/ItemDataTable.xlsx
+++ b/Assets/Data/ItemDataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuwonCha\SpartaCodingUnity\CampWeek8\MyUnityInventory\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0516A2ED-7388-41A6-BFE6-1A69AD6C8A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE735C7B-3CEB-4B4B-BBE2-DE25869B8ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{E92AB8CD-E172-45CE-AC0F-F9D22ECFD4F7}"/>
   </bookViews>
@@ -1194,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1217,7 +1217,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>